<commit_message>
fixing frontend design in adttendance table
</commit_message>
<xml_diff>
--- a/public/uploads/attendance_data_261361.xlsx
+++ b/public/uploads/attendance_data_261361.xlsx
@@ -397,17 +397,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="29.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -421,12 +420,9 @@
         <v>อีเมล</v>
       </c>
       <c r="D1" t="str">
-        <v>2025-03-06 - hw4</v>
+        <v>2025-03-13 - asdasdadaasd</v>
       </c>
       <c r="E1" t="str">
-        <v>2025-03-13</v>
-      </c>
-      <c r="F1" t="str">
         <v>23-01-2025 - HW1</v>
       </c>
     </row>
@@ -441,13 +437,10 @@
         <v>night@example.com</v>
       </c>
       <c r="D2" t="str">
-        <v>ขาดเรียน</v>
+        <v>0</v>
       </c>
       <c r="E2" t="str">
-        <v>ขาดเรียน</v>
-      </c>
-      <c r="F2" t="str">
-        <v>มาเรียน</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -461,98 +454,15 @@
         <v>earn@example.com</v>
       </c>
       <c r="D3" t="str">
-        <v>ขาดเรียน</v>
+        <v>0</v>
       </c>
       <c r="E3" t="str">
-        <v>ขาดเรียน</v>
-      </c>
-      <c r="F3" t="str">
-        <v>ขาดเรียน</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>650610763</v>
-      </c>
-      <c r="B4" t="str">
-        <v>aszrdhjlksfdhj;</v>
-      </c>
-      <c r="C4" t="str">
-        <v>itasfdjlks@cmu.ac.th</v>
-      </c>
-      <c r="D4" t="str">
-        <v>ขาดเรียน</v>
-      </c>
-      <c r="E4" t="str">
-        <v>ขาดเรียน</v>
-      </c>
-      <c r="F4" t="str">
-        <v>ขาดเรียน</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>065061076</v>
-      </c>
-      <c r="B5" t="str">
-        <v>aszrdhjlksfdhj;sda</v>
-      </c>
-      <c r="C5" t="str">
-        <v>itasfdzxcjlks@cmu.ac.th</v>
-      </c>
-      <c r="D5" t="str">
-        <v>ขาดเรียน</v>
-      </c>
-      <c r="E5" t="str">
-        <v>ขาดเรียน</v>
-      </c>
-      <c r="F5" t="str">
-        <v>ขาดเรียน</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>650610769</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Winney the pooh</v>
-      </c>
-      <c r="C6" t="str">
-        <v>azqwsexol@cmu.ac.th</v>
-      </c>
-      <c r="D6" t="str">
-        <v>ขาดเรียน</v>
-      </c>
-      <c r="E6" t="str">
-        <v>ขาดเรียน</v>
-      </c>
-      <c r="F6" t="str">
-        <v>ขาดเรียน</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>650610762</v>
-      </c>
-      <c r="B7" t="str">
-        <v>thiranat</v>
-      </c>
-      <c r="C7" t="str">
-        <v>thiranat_kakanmee@cmu.ac.th</v>
-      </c>
-      <c r="D7" t="str">
-        <v>มาเรียน</v>
-      </c>
-      <c r="E7" t="str">
-        <v>มาเรียน</v>
-      </c>
-      <c r="F7" t="str">
-        <v>ขาดเรียน</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>